<commit_message>
commit all java files
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/TestData.xlsx
+++ b/src/main/resources/Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkhare\git\VMS_Automation_TestNG_Cucumber\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4029E-FA66-4317-96C0-B7B1AB9C07C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4655B99D-A918-47F3-B056-82DE164BDE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>LRN</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Balerion@22</t>
+  </si>
+  <si>
+    <t>abhijeet.patil@prounlimited.com</t>
+  </si>
+  <si>
+    <t>qajupiter</t>
   </si>
   <si>
     <t>sunil.kumar@prounlimited.com</t>
@@ -578,10 +584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A0FDD4-DE88-45B7-A9C9-2B6BD3169885}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,13 +654,28 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{C40A6131-BDDE-4D7C-9543-A4D2D81F84EE}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{44089507-7046-4A11-B347-FC7D6AE470BF}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C8B870FB-E110-405B-A8AB-30D635D0FA01}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{6F1D03E4-9D21-4E12-A02C-F298768E3043}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>